<commit_message>
Implemented stock API, saving data to our Objects.
</commit_message>
<xml_diff>
--- a/artifacts/Ideas.xlsx
+++ b/artifacts/Ideas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_BootCamp\Projects\Group-Project-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_BootCamp\Projects\Group-Project-1\Stockman\stockman\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F5C26-E816-4E51-B284-11672883D4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF6B48D-4484-4AF3-8F47-F6E8881DC319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="2610" windowWidth="24705" windowHeight="11835" xr2:uid="{E8038AEF-AC3D-4573-82E2-8ADA9F290088}"/>
+    <workbookView xWindow="29175" yWindow="225" windowWidth="24705" windowHeight="11835" activeTab="1" xr2:uid="{E8038AEF-AC3D-4573-82E2-8ADA9F290088}"/>
   </bookViews>
   <sheets>
     <sheet name="Selection Page" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>Name:</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>Asset Score (FCAS)</t>
+  </si>
+  <si>
+    <t>(this one from AlpaAdvantage</t>
   </si>
 </sst>
 </file>
@@ -375,10 +381,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,8 +396,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -765,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A579B1-4918-4891-9ABF-02988F9BED89}">
   <dimension ref="A2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -800,25 +806,25 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -894,25 +900,25 @@
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="15" t="s">
         <v>22</v>
       </c>
     </row>
@@ -973,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC92FCB0-408D-4F89-8C6E-0A9AC83711A8}">
   <dimension ref="A2:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,15 +992,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1219,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA59454-9A88-4EB3-A75A-C28FF47DAF69}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,22 +1242,22 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1285,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>51</v>
       </c>
@@ -1296,14 +1302,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 'dailyCheck' logic and 'readme'
</commit_message>
<xml_diff>
--- a/artifacts/Ideas.xlsx
+++ b/artifacts/Ideas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_BootCamp\Projects\Group-Project-1\Stockman\stockman\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF6B48D-4484-4AF3-8F47-F6E8881DC319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD35AFB0-01B1-4539-8D0A-A55A15443D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29175" yWindow="225" windowWidth="24705" windowHeight="11835" activeTab="1" xr2:uid="{E8038AEF-AC3D-4573-82E2-8ADA9F290088}"/>
+    <workbookView xWindow="2475" yWindow="450" windowWidth="24705" windowHeight="14145" activeTab="2" xr2:uid="{E8038AEF-AC3D-4573-82E2-8ADA9F290088}"/>
   </bookViews>
   <sheets>
     <sheet name="Selection Page" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>Name:</t>
   </si>
@@ -50,9 +50,6 @@
     <t>EPS</t>
   </si>
   <si>
-    <t>Relative Strength</t>
-  </si>
-  <si>
     <t>PE</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t xml:space="preserve">https://coinmarketcap.com/ </t>
   </si>
   <si>
-    <t>Parameters to track</t>
-  </si>
-  <si>
     <t>Market Cap</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
     <t xml:space="preserve">https://www.fxempire.com/education/article/how-to-invest-in-cryptocurrencies-the-complete-guide-for-2020-651124 </t>
   </si>
   <si>
-    <t>Transaction Fee</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://blog.liquid.com/how-to-do-fundamental-analysis-for-cryptocurrency </t>
   </si>
   <si>
@@ -219,12 +210,6 @@
   </si>
   <si>
     <t>Currency</t>
-  </si>
-  <si>
-    <t>Asset Score (FCAS)</t>
-  </si>
-  <si>
-    <t>(this one from AlpaAdvantage</t>
   </si>
 </sst>
 </file>
@@ -420,13 +405,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -782,32 +767,32 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -819,7 +804,7 @@
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -828,16 +813,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -845,10 +830,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -856,10 +841,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -867,13 +852,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -881,10 +866,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -892,16 +877,16 @@
         <v>5</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -910,16 +895,16 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -927,10 +912,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -938,10 +923,10 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
         <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -949,10 +934,10 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
         <v>51</v>
-      </c>
-      <c r="D24" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -977,10 +962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC92FCB0-408D-4F89-8C6E-0A9AC83711A8}">
-  <dimension ref="A2:J31"/>
+  <dimension ref="A2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +978,7 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -1004,20 +989,20 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1025,26 +1010,26 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1065,15 +1050,15 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1081,16 +1066,16 @@
         <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="F20" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1098,29 +1083,29 @@
         <v>5</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" t="s">
         <v>39</v>
-      </c>
-      <c r="G21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1128,11 +1113,11 @@
         <v>6</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1140,11 +1125,11 @@
         <v>7</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1152,11 +1137,11 @@
         <v>8</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1164,11 +1149,11 @@
         <v>9</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1176,42 +1161,30 @@
         <v>10</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
       <c r="E30" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="13" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1225,99 +1198,109 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA59454-9A88-4EB3-A75A-C28FF47DAF69}">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>